<commit_message>
Work with Excel files. Part 12 (Restructure)
IReportService added. Setting file path improved.
</commit_message>
<xml_diff>
--- a/FitMeApp/wwwroot/ExcelFiles/Users.xlsx
+++ b/FitMeApp/wwwroot/ExcelFiles/Users.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users" sheetId="1" r:id="R8144774753694660"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users.xlsx" sheetId="1" r:id="Rd22a652c57d944d7"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -148,19 +148,19 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="1" t="str">
-        <x:v>User2</x:v>
+        <x:v>User5</x:v>
       </x:c>
       <x:c r="C4" s="1" t="str">
-        <x:v>LastUser2</x:v>
+        <x:v>User5LN</x:v>
       </x:c>
       <x:c r="D4" s="1" t="str">
-        <x:v>user2@gmail.com</x:v>
+        <x:v>user5@gmail.com</x:v>
       </x:c>
       <x:c r="E4" s="1" t="str">
-        <x:v>123456789</x:v>
+        <x:v>(159)753852</x:v>
       </x:c>
       <x:c r="F4" s="4" t="n">
-        <x:v>1923</x:v>
+        <x:v>2000</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
@@ -168,19 +168,19 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="1" t="str">
-        <x:v>Boxis</x:v>
+        <x:v>User2</x:v>
       </x:c>
       <x:c r="C5" s="1" t="str">
-        <x:v>Strong</x:v>
+        <x:v>LastUser2</x:v>
       </x:c>
       <x:c r="D5" s="1" t="str">
-        <x:v>boxis@gmail.com</x:v>
+        <x:v>user2@gmail.com</x:v>
       </x:c>
       <x:c r="E5" s="1" t="str">
-        <x:v>(111)333222</x:v>
+        <x:v>123456789</x:v>
       </x:c>
       <x:c r="F5" s="4" t="n">
-        <x:v>1993</x:v>
+        <x:v>1923</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
@@ -188,19 +188,19 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="B6" s="1" t="str">
-        <x:v>Tor</x:v>
+        <x:v>User8</x:v>
       </x:c>
       <x:c r="C6" s="1" t="str">
-        <x:v>Asgaard</x:v>
+        <x:v>User8LN</x:v>
       </x:c>
       <x:c r="D6" s="1" t="str">
-        <x:v>tor@gmail.com</x:v>
+        <x:v>user8@gmail.com</x:v>
       </x:c>
       <x:c r="E6" s="1" t="str">
-        <x:v>(111)333888</x:v>
+        <x:v>(159)753852</x:v>
       </x:c>
       <x:c r="F6" s="4" t="n">
-        <x:v>1994</x:v>
+        <x:v>2000</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
@@ -208,19 +208,19 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B7" s="1" t="str">
-        <x:v>Gunnar</x:v>
+        <x:v>Boxis</x:v>
       </x:c>
       <x:c r="C7" s="1" t="str">
-        <x:v>Jensen</x:v>
+        <x:v>Strong</x:v>
       </x:c>
       <x:c r="D7" s="1" t="str">
-        <x:v>gunnar@gmail.com</x:v>
+        <x:v>boxis@gmail.com</x:v>
       </x:c>
       <x:c r="E7" s="1" t="str">
-        <x:v>(111)222444</x:v>
+        <x:v>(111)333222</x:v>
       </x:c>
       <x:c r="F7" s="4" t="n">
-        <x:v>1980</x:v>
+        <x:v>1993</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
@@ -228,19 +228,19 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B8" s="1" t="str">
-        <x:v>Bruce</x:v>
+        <x:v>Tor</x:v>
       </x:c>
       <x:c r="C8" s="1" t="str">
-        <x:v>Lee</x:v>
+        <x:v>Asgaard</x:v>
       </x:c>
       <x:c r="D8" s="1" t="str">
-        <x:v>bruce@gmail.com</x:v>
+        <x:v>tor@gmail.com</x:v>
       </x:c>
       <x:c r="E8" s="1" t="str">
-        <x:v>(111)333445</x:v>
+        <x:v>(111)333888</x:v>
       </x:c>
       <x:c r="F8" s="4" t="n">
-        <x:v>1987</x:v>
+        <x:v>1994</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
@@ -248,19 +248,19 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B9" s="1" t="str">
-        <x:v>Gamora</x:v>
+        <x:v>User1</x:v>
       </x:c>
       <x:c r="C9" s="1" t="str">
-        <x:v>Gamorak</x:v>
+        <x:v>Admin1</x:v>
       </x:c>
       <x:c r="D9" s="1" t="str">
-        <x:v>gamora@gmail.com</x:v>
+        <x:v>user1@gmail.com</x:v>
       </x:c>
       <x:c r="E9" s="1" t="str">
-        <x:v>(111)333111</x:v>
+        <x:v>(123)456780</x:v>
       </x:c>
       <x:c r="F9" s="4" t="n">
-        <x:v>1988</x:v>
+        <x:v>1990</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
@@ -268,19 +268,19 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="B10" s="1" t="str">
-        <x:v>Witcher</x:v>
+        <x:v>Gunnar</x:v>
       </x:c>
       <x:c r="C10" s="1" t="str">
-        <x:v>Moon</x:v>
+        <x:v>Jensen</x:v>
       </x:c>
       <x:c r="D10" s="1" t="str">
-        <x:v>witcher@gmail.com</x:v>
+        <x:v>gunnar@gmail.com</x:v>
       </x:c>
       <x:c r="E10" s="1" t="str">
-        <x:v>(111)333999</x:v>
+        <x:v>(111)222444</x:v>
       </x:c>
       <x:c r="F10" s="4" t="n">
-        <x:v>1990</x:v>
+        <x:v>1980</x:v>
       </x:c>
     </x:row>
     <x:row r="11">
@@ -288,19 +288,19 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B11" s="1" t="str">
-        <x:v>Supwom</x:v>
+        <x:v>TestTrainer</x:v>
       </x:c>
       <x:c r="C11" s="1" t="str">
-        <x:v>Nanual</x:v>
+        <x:v>TeatTrainerLN</x:v>
       </x:c>
       <x:c r="D11" s="1" t="str">
-        <x:v>supwom@gmail.com</x:v>
+        <x:v>testTrainer@gmail.com</x:v>
       </x:c>
       <x:c r="E11" s="1" t="str">
-        <x:v>(111)333777</x:v>
+        <x:v>(123)123123</x:v>
       </x:c>
       <x:c r="F11" s="4" t="n">
-        <x:v>1988</x:v>
+        <x:v>1998</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
@@ -308,19 +308,19 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B12" s="1" t="str">
-        <x:v>Barney</x:v>
+        <x:v>Bruce</x:v>
       </x:c>
       <x:c r="C12" s="1" t="str">
-        <x:v>Ross</x:v>
+        <x:v>Lee</x:v>
       </x:c>
       <x:c r="D12" s="1" t="str">
-        <x:v>barney@gmail.com</x:v>
+        <x:v>bruce@gmail.com</x:v>
       </x:c>
       <x:c r="E12" s="1" t="str">
-        <x:v>(111)222333</x:v>
+        <x:v>(111)333445</x:v>
       </x:c>
       <x:c r="F12" s="4" t="n">
-        <x:v>1975</x:v>
+        <x:v>1987</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
@@ -328,19 +328,19 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B13" s="1" t="str">
-        <x:v>Lee</x:v>
+        <x:v>Gamora</x:v>
       </x:c>
       <x:c r="C13" s="1" t="str">
-        <x:v>Christmas</x:v>
+        <x:v>Gamorak</x:v>
       </x:c>
       <x:c r="D13" s="1" t="str">
-        <x:v>lee@gmail.com</x:v>
+        <x:v>gamora@gmail.com</x:v>
       </x:c>
       <x:c r="E13" s="1" t="str">
-        <x:v>(111)333444</x:v>
+        <x:v>(111)333111</x:v>
       </x:c>
       <x:c r="F13" s="4" t="n">
-        <x:v>1977</x:v>
+        <x:v>1988</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
@@ -348,19 +348,19 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="B14" s="1" t="str">
-        <x:v>Marvel</x:v>
+        <x:v>Witcher</x:v>
       </x:c>
       <x:c r="C14" s="1" t="str">
-        <x:v>Levram</x:v>
+        <x:v>Moon</x:v>
       </x:c>
       <x:c r="D14" s="1" t="str">
-        <x:v>marvel@gmail.com</x:v>
+        <x:v>witcher@gmail.com</x:v>
       </x:c>
       <x:c r="E14" s="1" t="str">
-        <x:v>(111)333555</x:v>
+        <x:v>(111)333999</x:v>
       </x:c>
       <x:c r="F14" s="4" t="n">
-        <x:v>1995</x:v>
+        <x:v>1990</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
@@ -368,19 +368,19 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="B15" s="1" t="str">
-        <x:v>Jean</x:v>
+        <x:v>Supwom</x:v>
       </x:c>
       <x:c r="C15" s="1" t="str">
-        <x:v>Vilain</x:v>
+        <x:v>Nanual</x:v>
       </x:c>
       <x:c r="D15" s="1" t="str">
-        <x:v>jean@gmail.com</x:v>
+        <x:v>supwom@gmail.com</x:v>
       </x:c>
       <x:c r="E15" s="1" t="str">
-        <x:v>(111)222777</x:v>
+        <x:v>(111)333777</x:v>
       </x:c>
       <x:c r="F15" s="4" t="n">
-        <x:v>1973</x:v>
+        <x:v>1988</x:v>
       </x:c>
     </x:row>
     <x:row r="16">
@@ -388,19 +388,19 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="B16" s="1" t="str">
-        <x:v>Sonya</x:v>
+        <x:v>Barney</x:v>
       </x:c>
       <x:c r="C16" s="1" t="str">
-        <x:v>Night</x:v>
+        <x:v>Ross</x:v>
       </x:c>
       <x:c r="D16" s="1" t="str">
-        <x:v>sonya@gmail.com</x:v>
+        <x:v>barney@gmail.com</x:v>
       </x:c>
       <x:c r="E16" s="1" t="str">
-        <x:v>(111)333666</x:v>
+        <x:v>(111)222333</x:v>
       </x:c>
       <x:c r="F16" s="4" t="n">
-        <x:v>1996</x:v>
+        <x:v>1975</x:v>
       </x:c>
     </x:row>
     <x:row r="17">
@@ -408,18 +408,118 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B17" s="1" t="str">
+        <x:v>Lee</x:v>
+      </x:c>
+      <x:c r="C17" s="1" t="str">
+        <x:v>Christmas</x:v>
+      </x:c>
+      <x:c r="D17" s="1" t="str">
+        <x:v>lee@gmail.com</x:v>
+      </x:c>
+      <x:c r="E17" s="1" t="str">
+        <x:v>(111)333444</x:v>
+      </x:c>
+      <x:c r="F17" s="4" t="n">
+        <x:v>1977</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18">
+      <x:c r="A18" s="4" t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B18" s="1" t="str">
+        <x:v>Marvel</x:v>
+      </x:c>
+      <x:c r="C18" s="1" t="str">
+        <x:v>Levram</x:v>
+      </x:c>
+      <x:c r="D18" s="1" t="str">
+        <x:v>marvel@gmail.com</x:v>
+      </x:c>
+      <x:c r="E18" s="1" t="str">
+        <x:v>(111)333555</x:v>
+      </x:c>
+      <x:c r="F18" s="4" t="n">
+        <x:v>1995</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19">
+      <x:c r="A19" s="4" t="n">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B19" s="1" t="str">
+        <x:v>Jean</x:v>
+      </x:c>
+      <x:c r="C19" s="1" t="str">
+        <x:v>Vilain</x:v>
+      </x:c>
+      <x:c r="D19" s="1" t="str">
+        <x:v>jean@gmail.com</x:v>
+      </x:c>
+      <x:c r="E19" s="1" t="str">
+        <x:v>(111)222777</x:v>
+      </x:c>
+      <x:c r="F19" s="4" t="n">
+        <x:v>1973</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20">
+      <x:c r="A20" s="4" t="n">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B20" s="1" t="str">
+        <x:v>User6</x:v>
+      </x:c>
+      <x:c r="C20" s="1" t="str">
+        <x:v>User6LN</x:v>
+      </x:c>
+      <x:c r="D20" s="1" t="str">
+        <x:v>user6@gmail.com</x:v>
+      </x:c>
+      <x:c r="E20" s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="F20" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21">
+      <x:c r="A21" s="4" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B21" s="1" t="str">
+        <x:v>Sonya</x:v>
+      </x:c>
+      <x:c r="C21" s="1" t="str">
+        <x:v>Night</x:v>
+      </x:c>
+      <x:c r="D21" s="1" t="str">
+        <x:v>sonya@gmail.com</x:v>
+      </x:c>
+      <x:c r="E21" s="1" t="str">
+        <x:v>(111)333666</x:v>
+      </x:c>
+      <x:c r="F21" s="4" t="n">
+        <x:v>1996</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22">
+      <x:c r="A22" s="4" t="n">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B22" s="1" t="str">
         <x:v>Natalia</x:v>
       </x:c>
-      <x:c r="C17" s="1" t="str">
+      <x:c r="C22" s="1" t="str">
         <x:v>Romanoff</x:v>
       </x:c>
-      <x:c r="D17" s="1" t="str">
+      <x:c r="D22" s="1" t="str">
         <x:v>natalia@gmail.com</x:v>
       </x:c>
-      <x:c r="E17" s="1" t="str">
+      <x:c r="E22" s="1" t="str">
         <x:v>(111)222888</x:v>
       </x:c>
-      <x:c r="F17" s="4" t="n">
+      <x:c r="F22" s="4" t="n">
         <x:v>1986</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Read data from Excel. Part 1 (EPPlus realization)
</commit_message>
<xml_diff>
--- a/FitMeApp/wwwroot/ExcelFiles/Users.xlsx
+++ b/FitMeApp/wwwroot/ExcelFiles/Users.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users.xlsx" sheetId="1" r:id="Rd22a652c57d944d7"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users.xlsx" sheetId="1" r:id="R502f37521ed74f49"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -28,7 +28,7 @@
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
-        <x:fgColor rgb="66666666"/>
+        <x:fgColor rgb="93d19f"/>
       </x:patternFill>
     </x:fill>
   </x:fills>

</xml_diff>

<commit_message>
WriteToExcelAsync method (OpenXml realization) fixed. Small fixes
Distenation path for Users.xlsx added to recources.
</commit_message>
<xml_diff>
--- a/FitMeApp/wwwroot/ExcelFiles/Users.xlsx
+++ b/FitMeApp/wwwroot/ExcelFiles/Users.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users.xlsx" sheetId="1" r:id="R502f37521ed74f49"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users.xlsx" sheetId="1" r:id="R8fe8aa32e92b4e12"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -288,19 +288,19 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B11" s="1" t="str">
-        <x:v>TestTrainer</x:v>
+        <x:v>Bruce</x:v>
       </x:c>
       <x:c r="C11" s="1" t="str">
-        <x:v>TeatTrainerLN</x:v>
+        <x:v>Lee</x:v>
       </x:c>
       <x:c r="D11" s="1" t="str">
-        <x:v>testTrainer@gmail.com</x:v>
+        <x:v>bruce@gmail.com</x:v>
       </x:c>
       <x:c r="E11" s="1" t="str">
-        <x:v>(123)123123</x:v>
+        <x:v>(111)333445</x:v>
       </x:c>
       <x:c r="F11" s="4" t="n">
-        <x:v>1998</x:v>
+        <x:v>1987</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
@@ -308,19 +308,19 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B12" s="1" t="str">
-        <x:v>Bruce</x:v>
+        <x:v>Gamora</x:v>
       </x:c>
       <x:c r="C12" s="1" t="str">
-        <x:v>Lee</x:v>
+        <x:v>Gamorak</x:v>
       </x:c>
       <x:c r="D12" s="1" t="str">
-        <x:v>bruce@gmail.com</x:v>
+        <x:v>gamora@gmail.com</x:v>
       </x:c>
       <x:c r="E12" s="1" t="str">
-        <x:v>(111)333445</x:v>
+        <x:v>(111)333111</x:v>
       </x:c>
       <x:c r="F12" s="4" t="n">
-        <x:v>1987</x:v>
+        <x:v>1988</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
@@ -328,19 +328,19 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B13" s="1" t="str">
-        <x:v>Gamora</x:v>
+        <x:v>Witcher</x:v>
       </x:c>
       <x:c r="C13" s="1" t="str">
-        <x:v>Gamorak</x:v>
+        <x:v>Moon</x:v>
       </x:c>
       <x:c r="D13" s="1" t="str">
-        <x:v>gamora@gmail.com</x:v>
+        <x:v>witcher@gmail.com</x:v>
       </x:c>
       <x:c r="E13" s="1" t="str">
-        <x:v>(111)333111</x:v>
+        <x:v>(111)333999</x:v>
       </x:c>
       <x:c r="F13" s="4" t="n">
-        <x:v>1988</x:v>
+        <x:v>1990</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
@@ -348,19 +348,19 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="B14" s="1" t="str">
-        <x:v>Witcher</x:v>
+        <x:v>Supwom</x:v>
       </x:c>
       <x:c r="C14" s="1" t="str">
-        <x:v>Moon</x:v>
+        <x:v>Nanual</x:v>
       </x:c>
       <x:c r="D14" s="1" t="str">
-        <x:v>witcher@gmail.com</x:v>
+        <x:v>supwom@gmail.com</x:v>
       </x:c>
       <x:c r="E14" s="1" t="str">
-        <x:v>(111)333999</x:v>
+        <x:v>(111)333777</x:v>
       </x:c>
       <x:c r="F14" s="4" t="n">
-        <x:v>1990</x:v>
+        <x:v>1988</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
@@ -368,19 +368,19 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="B15" s="1" t="str">
-        <x:v>Supwom</x:v>
+        <x:v>Barney</x:v>
       </x:c>
       <x:c r="C15" s="1" t="str">
-        <x:v>Nanual</x:v>
+        <x:v>Ross</x:v>
       </x:c>
       <x:c r="D15" s="1" t="str">
-        <x:v>supwom@gmail.com</x:v>
+        <x:v>barney@gmail.com</x:v>
       </x:c>
       <x:c r="E15" s="1" t="str">
-        <x:v>(111)333777</x:v>
+        <x:v>(111)222333</x:v>
       </x:c>
       <x:c r="F15" s="4" t="n">
-        <x:v>1988</x:v>
+        <x:v>1975</x:v>
       </x:c>
     </x:row>
     <x:row r="16">
@@ -388,19 +388,19 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="B16" s="1" t="str">
-        <x:v>Barney</x:v>
+        <x:v>Lee</x:v>
       </x:c>
       <x:c r="C16" s="1" t="str">
-        <x:v>Ross</x:v>
+        <x:v>Christmas</x:v>
       </x:c>
       <x:c r="D16" s="1" t="str">
-        <x:v>barney@gmail.com</x:v>
+        <x:v>lee@gmail.com</x:v>
       </x:c>
       <x:c r="E16" s="1" t="str">
-        <x:v>(111)222333</x:v>
+        <x:v>(111)333444</x:v>
       </x:c>
       <x:c r="F16" s="4" t="n">
-        <x:v>1975</x:v>
+        <x:v>1977</x:v>
       </x:c>
     </x:row>
     <x:row r="17">
@@ -408,19 +408,19 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B17" s="1" t="str">
-        <x:v>Lee</x:v>
+        <x:v>Marvel</x:v>
       </x:c>
       <x:c r="C17" s="1" t="str">
-        <x:v>Christmas</x:v>
+        <x:v>Levram</x:v>
       </x:c>
       <x:c r="D17" s="1" t="str">
-        <x:v>lee@gmail.com</x:v>
+        <x:v>marvel@gmail.com</x:v>
       </x:c>
       <x:c r="E17" s="1" t="str">
-        <x:v>(111)333444</x:v>
+        <x:v>(111)333555</x:v>
       </x:c>
       <x:c r="F17" s="4" t="n">
-        <x:v>1977</x:v>
+        <x:v>1995</x:v>
       </x:c>
     </x:row>
     <x:row r="18">
@@ -428,19 +428,19 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="B18" s="1" t="str">
-        <x:v>Marvel</x:v>
+        <x:v>Jean</x:v>
       </x:c>
       <x:c r="C18" s="1" t="str">
-        <x:v>Levram</x:v>
+        <x:v>Vilain</x:v>
       </x:c>
       <x:c r="D18" s="1" t="str">
-        <x:v>marvel@gmail.com</x:v>
+        <x:v>jean@gmail.com</x:v>
       </x:c>
       <x:c r="E18" s="1" t="str">
-        <x:v>(111)333555</x:v>
+        <x:v>(111)222777</x:v>
       </x:c>
       <x:c r="F18" s="4" t="n">
-        <x:v>1995</x:v>
+        <x:v>1973</x:v>
       </x:c>
     </x:row>
     <x:row r="19">
@@ -448,19 +448,19 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="B19" s="1" t="str">
-        <x:v>Jean</x:v>
+        <x:v>User6</x:v>
       </x:c>
       <x:c r="C19" s="1" t="str">
-        <x:v>Vilain</x:v>
+        <x:v>User6LN</x:v>
       </x:c>
       <x:c r="D19" s="1" t="str">
-        <x:v>jean@gmail.com</x:v>
+        <x:v>user6@gmail.com</x:v>
       </x:c>
       <x:c r="E19" s="1" t="str">
-        <x:v>(111)222777</x:v>
+        <x:v/>
       </x:c>
       <x:c r="F19" s="4" t="n">
-        <x:v>1973</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="20">
@@ -468,19 +468,19 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="B20" s="1" t="str">
-        <x:v>User6</x:v>
+        <x:v>Sonya</x:v>
       </x:c>
       <x:c r="C20" s="1" t="str">
-        <x:v>User6LN</x:v>
+        <x:v>Night</x:v>
       </x:c>
       <x:c r="D20" s="1" t="str">
-        <x:v>user6@gmail.com</x:v>
+        <x:v>sonya@gmail.com</x:v>
       </x:c>
       <x:c r="E20" s="1" t="str">
-        <x:v/>
+        <x:v>(111)333666</x:v>
       </x:c>
       <x:c r="F20" s="4" t="n">
-        <x:v>0</x:v>
+        <x:v>1996</x:v>
       </x:c>
     </x:row>
     <x:row r="21">
@@ -488,38 +488,18 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="B21" s="1" t="str">
-        <x:v>Sonya</x:v>
+        <x:v>Natalia</x:v>
       </x:c>
       <x:c r="C21" s="1" t="str">
-        <x:v>Night</x:v>
+        <x:v>Romanoff</x:v>
       </x:c>
       <x:c r="D21" s="1" t="str">
-        <x:v>sonya@gmail.com</x:v>
+        <x:v>natalia@gmail.com</x:v>
       </x:c>
       <x:c r="E21" s="1" t="str">
-        <x:v>(111)333666</x:v>
+        <x:v>(111)222888</x:v>
       </x:c>
       <x:c r="F21" s="4" t="n">
-        <x:v>1996</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22">
-      <x:c r="A22" s="4" t="n">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="B22" s="1" t="str">
-        <x:v>Natalia</x:v>
-      </x:c>
-      <x:c r="C22" s="1" t="str">
-        <x:v>Romanoff</x:v>
-      </x:c>
-      <x:c r="D22" s="1" t="str">
-        <x:v>natalia@gmail.com</x:v>
-      </x:c>
-      <x:c r="E22" s="1" t="str">
-        <x:v>(111)222888</x:v>
-      </x:c>
-      <x:c r="F22" s="4" t="n">
         <x:v>1986</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Resources access has been changed
</commit_message>
<xml_diff>
--- a/FitMeApp/wwwroot/ExcelFiles/Users.xlsx
+++ b/FitMeApp/wwwroot/ExcelFiles/Users.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users.xlsx" sheetId="1" r:id="R8fe8aa32e92b4e12"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users.xlsx" sheetId="1" r:id="R74afb3dbfef94acb"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -148,16 +148,16 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="1" t="str">
-        <x:v>User5</x:v>
+        <x:v>User6</x:v>
       </x:c>
       <x:c r="C4" s="1" t="str">
-        <x:v>User5LN</x:v>
+        <x:v>User6LN</x:v>
       </x:c>
       <x:c r="D4" s="1" t="str">
-        <x:v>user5@gmail.com</x:v>
+        <x:v>user6@gmail.com</x:v>
       </x:c>
       <x:c r="E4" s="1" t="str">
-        <x:v>(159)753852</x:v>
+        <x:v>123987654</x:v>
       </x:c>
       <x:c r="F4" s="4" t="n">
         <x:v>2000</x:v>
@@ -168,19 +168,19 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="1" t="str">
-        <x:v>User2</x:v>
+        <x:v>User4</x:v>
       </x:c>
       <x:c r="C5" s="1" t="str">
-        <x:v>LastUser2</x:v>
+        <x:v>User4LN</x:v>
       </x:c>
       <x:c r="D5" s="1" t="str">
-        <x:v>user2@gmail.com</x:v>
+        <x:v>user4@gmail.com</x:v>
       </x:c>
       <x:c r="E5" s="1" t="str">
-        <x:v>123456789</x:v>
+        <x:v>(123)123456789</x:v>
       </x:c>
       <x:c r="F5" s="4" t="n">
-        <x:v>1923</x:v>
+        <x:v>2000</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
@@ -188,19 +188,19 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="B6" s="1" t="str">
-        <x:v>User8</x:v>
+        <x:v>Boxis</x:v>
       </x:c>
       <x:c r="C6" s="1" t="str">
-        <x:v>User8LN</x:v>
+        <x:v>Strong</x:v>
       </x:c>
       <x:c r="D6" s="1" t="str">
-        <x:v>user8@gmail.com</x:v>
+        <x:v>boxis@gmail.com</x:v>
       </x:c>
       <x:c r="E6" s="1" t="str">
-        <x:v>(159)753852</x:v>
+        <x:v>(111)333222</x:v>
       </x:c>
       <x:c r="F6" s="4" t="n">
-        <x:v>2000</x:v>
+        <x:v>1993</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
@@ -208,19 +208,19 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B7" s="1" t="str">
-        <x:v>Boxis</x:v>
+        <x:v>Tor</x:v>
       </x:c>
       <x:c r="C7" s="1" t="str">
-        <x:v>Strong</x:v>
+        <x:v>Asgaard</x:v>
       </x:c>
       <x:c r="D7" s="1" t="str">
-        <x:v>boxis@gmail.com</x:v>
+        <x:v>tor@gmail.com</x:v>
       </x:c>
       <x:c r="E7" s="1" t="str">
-        <x:v>(111)333222</x:v>
+        <x:v>(111)333888</x:v>
       </x:c>
       <x:c r="F7" s="4" t="n">
-        <x:v>1993</x:v>
+        <x:v>1994</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
@@ -228,19 +228,19 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B8" s="1" t="str">
-        <x:v>Tor</x:v>
+        <x:v>User1</x:v>
       </x:c>
       <x:c r="C8" s="1" t="str">
-        <x:v>Asgaard</x:v>
+        <x:v>Admin1</x:v>
       </x:c>
       <x:c r="D8" s="1" t="str">
-        <x:v>tor@gmail.com</x:v>
+        <x:v>user1@gmail.com</x:v>
       </x:c>
       <x:c r="E8" s="1" t="str">
-        <x:v>(111)333888</x:v>
+        <x:v>(123)456780</x:v>
       </x:c>
       <x:c r="F8" s="4" t="n">
-        <x:v>1994</x:v>
+        <x:v>1990</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
@@ -248,19 +248,19 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B9" s="1" t="str">
-        <x:v>User1</x:v>
+        <x:v>Gunnar</x:v>
       </x:c>
       <x:c r="C9" s="1" t="str">
-        <x:v>Admin1</x:v>
+        <x:v>Jensen</x:v>
       </x:c>
       <x:c r="D9" s="1" t="str">
-        <x:v>user1@gmail.com</x:v>
+        <x:v>gunnar@gmail.com</x:v>
       </x:c>
       <x:c r="E9" s="1" t="str">
-        <x:v>(123)456780</x:v>
+        <x:v>(111)222444</x:v>
       </x:c>
       <x:c r="F9" s="4" t="n">
-        <x:v>1990</x:v>
+        <x:v>1980</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
@@ -268,19 +268,19 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="B10" s="1" t="str">
-        <x:v>Gunnar</x:v>
+        <x:v>Bruce</x:v>
       </x:c>
       <x:c r="C10" s="1" t="str">
-        <x:v>Jensen</x:v>
+        <x:v>Lee</x:v>
       </x:c>
       <x:c r="D10" s="1" t="str">
-        <x:v>gunnar@gmail.com</x:v>
+        <x:v>bruce@gmail.com</x:v>
       </x:c>
       <x:c r="E10" s="1" t="str">
-        <x:v>(111)222444</x:v>
+        <x:v>(111)333445</x:v>
       </x:c>
       <x:c r="F10" s="4" t="n">
-        <x:v>1980</x:v>
+        <x:v>1987</x:v>
       </x:c>
     </x:row>
     <x:row r="11">
@@ -288,19 +288,19 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B11" s="1" t="str">
-        <x:v>Bruce</x:v>
+        <x:v>Gamora</x:v>
       </x:c>
       <x:c r="C11" s="1" t="str">
-        <x:v>Lee</x:v>
+        <x:v>Gamorak</x:v>
       </x:c>
       <x:c r="D11" s="1" t="str">
-        <x:v>bruce@gmail.com</x:v>
+        <x:v>gamora@gmail.com</x:v>
       </x:c>
       <x:c r="E11" s="1" t="str">
-        <x:v>(111)333445</x:v>
+        <x:v>(111)333111</x:v>
       </x:c>
       <x:c r="F11" s="4" t="n">
-        <x:v>1987</x:v>
+        <x:v>1988</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
@@ -308,19 +308,19 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B12" s="1" t="str">
-        <x:v>Gamora</x:v>
+        <x:v>Witcher</x:v>
       </x:c>
       <x:c r="C12" s="1" t="str">
-        <x:v>Gamorak</x:v>
+        <x:v>Moon</x:v>
       </x:c>
       <x:c r="D12" s="1" t="str">
-        <x:v>gamora@gmail.com</x:v>
+        <x:v>witcher@gmail.com</x:v>
       </x:c>
       <x:c r="E12" s="1" t="str">
-        <x:v>(111)333111</x:v>
+        <x:v>(111)333999</x:v>
       </x:c>
       <x:c r="F12" s="4" t="n">
-        <x:v>1988</x:v>
+        <x:v>1990</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
@@ -328,19 +328,19 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B13" s="1" t="str">
-        <x:v>Witcher</x:v>
+        <x:v>Supwom</x:v>
       </x:c>
       <x:c r="C13" s="1" t="str">
-        <x:v>Moon</x:v>
+        <x:v>Nanual</x:v>
       </x:c>
       <x:c r="D13" s="1" t="str">
-        <x:v>witcher@gmail.com</x:v>
+        <x:v>supwom@gmail.com</x:v>
       </x:c>
       <x:c r="E13" s="1" t="str">
-        <x:v>(111)333999</x:v>
+        <x:v>(111)333777</x:v>
       </x:c>
       <x:c r="F13" s="4" t="n">
-        <x:v>1990</x:v>
+        <x:v>1988</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
@@ -348,19 +348,19 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="B14" s="1" t="str">
-        <x:v>Supwom</x:v>
+        <x:v>User5</x:v>
       </x:c>
       <x:c r="C14" s="1" t="str">
-        <x:v>Nanual</x:v>
+        <x:v>User5LN</x:v>
       </x:c>
       <x:c r="D14" s="1" t="str">
-        <x:v>supwom@gmail.com</x:v>
+        <x:v>user5@gmail.com</x:v>
       </x:c>
       <x:c r="E14" s="1" t="str">
-        <x:v>(111)333777</x:v>
+        <x:v/>
       </x:c>
       <x:c r="F14" s="4" t="n">
-        <x:v>1988</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
@@ -388,19 +388,19 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="B16" s="1" t="str">
-        <x:v>Lee</x:v>
+        <x:v>User2</x:v>
       </x:c>
       <x:c r="C16" s="1" t="str">
-        <x:v>Christmas</x:v>
+        <x:v>User2LN</x:v>
       </x:c>
       <x:c r="D16" s="1" t="str">
-        <x:v>lee@gmail.com</x:v>
+        <x:v>user2@gmail.com</x:v>
       </x:c>
       <x:c r="E16" s="1" t="str">
-        <x:v>(111)333444</x:v>
+        <x:v>(123)123123</x:v>
       </x:c>
       <x:c r="F16" s="4" t="n">
-        <x:v>1977</x:v>
+        <x:v>1995</x:v>
       </x:c>
     </x:row>
     <x:row r="17">
@@ -408,19 +408,19 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="B17" s="1" t="str">
-        <x:v>Marvel</x:v>
+        <x:v>Lee</x:v>
       </x:c>
       <x:c r="C17" s="1" t="str">
-        <x:v>Levram</x:v>
+        <x:v>Christmas</x:v>
       </x:c>
       <x:c r="D17" s="1" t="str">
-        <x:v>marvel@gmail.com</x:v>
+        <x:v>lee@gmail.com</x:v>
       </x:c>
       <x:c r="E17" s="1" t="str">
-        <x:v>(111)333555</x:v>
+        <x:v>(111)333444</x:v>
       </x:c>
       <x:c r="F17" s="4" t="n">
-        <x:v>1995</x:v>
+        <x:v>1977</x:v>
       </x:c>
     </x:row>
     <x:row r="18">
@@ -428,19 +428,19 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="B18" s="1" t="str">
-        <x:v>Jean</x:v>
+        <x:v>User3</x:v>
       </x:c>
       <x:c r="C18" s="1" t="str">
-        <x:v>Vilain</x:v>
+        <x:v>User3LN</x:v>
       </x:c>
       <x:c r="D18" s="1" t="str">
-        <x:v>jean@gmail.com</x:v>
+        <x:v>user3@gmail.com</x:v>
       </x:c>
       <x:c r="E18" s="1" t="str">
-        <x:v>(111)222777</x:v>
+        <x:v>(123)123124</x:v>
       </x:c>
       <x:c r="F18" s="4" t="n">
-        <x:v>1973</x:v>
+        <x:v>1996</x:v>
       </x:c>
     </x:row>
     <x:row r="19">
@@ -448,19 +448,19 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="B19" s="1" t="str">
-        <x:v>User6</x:v>
+        <x:v>Marvel</x:v>
       </x:c>
       <x:c r="C19" s="1" t="str">
-        <x:v>User6LN</x:v>
+        <x:v>Levram</x:v>
       </x:c>
       <x:c r="D19" s="1" t="str">
-        <x:v>user6@gmail.com</x:v>
+        <x:v>marvel@gmail.com</x:v>
       </x:c>
       <x:c r="E19" s="1" t="str">
-        <x:v/>
+        <x:v>(111)333555</x:v>
       </x:c>
       <x:c r="F19" s="4" t="n">
-        <x:v>0</x:v>
+        <x:v>1995</x:v>
       </x:c>
     </x:row>
     <x:row r="20">
@@ -468,19 +468,19 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="B20" s="1" t="str">
-        <x:v>Sonya</x:v>
+        <x:v>Jean</x:v>
       </x:c>
       <x:c r="C20" s="1" t="str">
-        <x:v>Night</x:v>
+        <x:v>Vilain</x:v>
       </x:c>
       <x:c r="D20" s="1" t="str">
-        <x:v>sonya@gmail.com</x:v>
+        <x:v>jean@gmail.com</x:v>
       </x:c>
       <x:c r="E20" s="1" t="str">
-        <x:v>(111)333666</x:v>
+        <x:v>(111)222777</x:v>
       </x:c>
       <x:c r="F20" s="4" t="n">
-        <x:v>1996</x:v>
+        <x:v>1973</x:v>
       </x:c>
     </x:row>
     <x:row r="21">
@@ -488,18 +488,38 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="B21" s="1" t="str">
+        <x:v>Sonya</x:v>
+      </x:c>
+      <x:c r="C21" s="1" t="str">
+        <x:v>Night</x:v>
+      </x:c>
+      <x:c r="D21" s="1" t="str">
+        <x:v>sonya@gmail.com</x:v>
+      </x:c>
+      <x:c r="E21" s="1" t="str">
+        <x:v>(111)333666</x:v>
+      </x:c>
+      <x:c r="F21" s="4" t="n">
+        <x:v>1996</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22">
+      <x:c r="A22" s="4" t="n">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B22" s="1" t="str">
         <x:v>Natalia</x:v>
       </x:c>
-      <x:c r="C21" s="1" t="str">
+      <x:c r="C22" s="1" t="str">
         <x:v>Romanoff</x:v>
       </x:c>
-      <x:c r="D21" s="1" t="str">
+      <x:c r="D22" s="1" t="str">
         <x:v>natalia@gmail.com</x:v>
       </x:c>
-      <x:c r="E21" s="1" t="str">
+      <x:c r="E22" s="1" t="str">
         <x:v>(111)222888</x:v>
       </x:c>
-      <x:c r="F21" s="4" t="n">
+      <x:c r="F22" s="4" t="n">
         <x:v>1986</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Restructure FileService and ReportService
</commit_message>
<xml_diff>
--- a/FitMeApp/wwwroot/ExcelFiles/Users.xlsx
+++ b/FitMeApp/wwwroot/ExcelFiles/Users.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users.xlsx" sheetId="1" r:id="R451bf56ba57444f3"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users.xlsx" sheetId="1" r:id="Rc5b5b1147a1c434f"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -108,19 +108,19 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="1" t="str">
-        <x:v>Boxis</x:v>
+        <x:v>Terry</x:v>
       </x:c>
       <x:c r="C2" s="1" t="str">
-        <x:v>Strong</x:v>
+        <x:v>Caesar</x:v>
       </x:c>
       <x:c r="D2" s="1" t="str">
-        <x:v>boxis@gmail.com</x:v>
+        <x:v>terry@gmail.com</x:v>
       </x:c>
       <x:c r="E2" s="1" t="str">
-        <x:v>(111)333222</x:v>
+        <x:v>(111)222666</x:v>
       </x:c>
       <x:c r="F2" s="4" t="n">
-        <x:v>1993</x:v>
+        <x:v>1983</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
@@ -128,19 +128,19 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="1" t="str">
-        <x:v>Barney</x:v>
+        <x:v>Wanda</x:v>
       </x:c>
       <x:c r="C3" s="1" t="str">
-        <x:v>Ross</x:v>
+        <x:v>Maximoff</x:v>
       </x:c>
       <x:c r="D3" s="1" t="str">
-        <x:v>barney@gmail.com</x:v>
+        <x:v>wanda@gmail.com</x:v>
       </x:c>
       <x:c r="E3" s="1" t="str">
-        <x:v>(111)222333</x:v>
+        <x:v>(111)222999</x:v>
       </x:c>
       <x:c r="F3" s="4" t="n">
-        <x:v>1975</x:v>
+        <x:v>1990</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
@@ -148,19 +148,399 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="1" t="str">
+        <x:v>User6</x:v>
+      </x:c>
+      <x:c r="C4" s="1" t="str">
+        <x:v>User6LN</x:v>
+      </x:c>
+      <x:c r="D4" s="1" t="str">
+        <x:v>user6@gmail.com</x:v>
+      </x:c>
+      <x:c r="E4" s="1" t="str">
+        <x:v>123987654</x:v>
+      </x:c>
+      <x:c r="F4" s="4" t="n">
+        <x:v>2000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5">
+      <x:c r="A5" s="4" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B5" s="1" t="str">
+        <x:v>User4</x:v>
+      </x:c>
+      <x:c r="C5" s="1" t="str">
+        <x:v>User4LN</x:v>
+      </x:c>
+      <x:c r="D5" s="1" t="str">
+        <x:v>user4@gmail.com</x:v>
+      </x:c>
+      <x:c r="E5" s="1" t="str">
+        <x:v>(123)123456789</x:v>
+      </x:c>
+      <x:c r="F5" s="4" t="n">
+        <x:v>2000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6">
+      <x:c r="A6" s="4" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B6" s="1" t="str">
+        <x:v>User7</x:v>
+      </x:c>
+      <x:c r="C6" s="1" t="str">
+        <x:v>User7LN</x:v>
+      </x:c>
+      <x:c r="D6" s="1" t="str">
+        <x:v>user7@gmail.com</x:v>
+      </x:c>
+      <x:c r="E6" s="1" t="str">
+        <x:v>(123)123123</x:v>
+      </x:c>
+      <x:c r="F6" s="4" t="n">
+        <x:v>1995</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7">
+      <x:c r="A7" s="4" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B7" s="1" t="str">
+        <x:v>Boxis</x:v>
+      </x:c>
+      <x:c r="C7" s="1" t="str">
+        <x:v>Strong</x:v>
+      </x:c>
+      <x:c r="D7" s="1" t="str">
+        <x:v>boxis@gmail.com</x:v>
+      </x:c>
+      <x:c r="E7" s="1" t="str">
+        <x:v>(111)333222</x:v>
+      </x:c>
+      <x:c r="F7" s="4" t="n">
+        <x:v>1993</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8">
+      <x:c r="A8" s="4" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B8" s="1" t="str">
+        <x:v>Tor</x:v>
+      </x:c>
+      <x:c r="C8" s="1" t="str">
+        <x:v>Asgaard</x:v>
+      </x:c>
+      <x:c r="D8" s="1" t="str">
+        <x:v>tor@gmail.com</x:v>
+      </x:c>
+      <x:c r="E8" s="1" t="str">
+        <x:v>(111)333888</x:v>
+      </x:c>
+      <x:c r="F8" s="4" t="n">
+        <x:v>1994</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9">
+      <x:c r="A9" s="4" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B9" s="1" t="str">
+        <x:v>User1</x:v>
+      </x:c>
+      <x:c r="C9" s="1" t="str">
+        <x:v>Admin1</x:v>
+      </x:c>
+      <x:c r="D9" s="1" t="str">
+        <x:v>user1@gmail.com</x:v>
+      </x:c>
+      <x:c r="E9" s="1" t="str">
+        <x:v>(123)456780</x:v>
+      </x:c>
+      <x:c r="F9" s="4" t="n">
+        <x:v>1990</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10">
+      <x:c r="A10" s="4" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B10" s="1" t="str">
+        <x:v>Gunnar</x:v>
+      </x:c>
+      <x:c r="C10" s="1" t="str">
+        <x:v>Jensen</x:v>
+      </x:c>
+      <x:c r="D10" s="1" t="str">
+        <x:v>gunnar@gmail.com</x:v>
+      </x:c>
+      <x:c r="E10" s="1" t="str">
+        <x:v>(111)222444</x:v>
+      </x:c>
+      <x:c r="F10" s="4" t="n">
+        <x:v>1980</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11">
+      <x:c r="A11" s="4" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B11" s="1" t="str">
+        <x:v>Bruce</x:v>
+      </x:c>
+      <x:c r="C11" s="1" t="str">
+        <x:v>Lee</x:v>
+      </x:c>
+      <x:c r="D11" s="1" t="str">
+        <x:v>bruce@gmail.com</x:v>
+      </x:c>
+      <x:c r="E11" s="1" t="str">
+        <x:v>(111)333445</x:v>
+      </x:c>
+      <x:c r="F11" s="4" t="n">
+        <x:v>1987</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12">
+      <x:c r="A12" s="4" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B12" s="1" t="str">
+        <x:v>Gamora</x:v>
+      </x:c>
+      <x:c r="C12" s="1" t="str">
+        <x:v>Gamorak</x:v>
+      </x:c>
+      <x:c r="D12" s="1" t="str">
+        <x:v>gamora@gmail.com</x:v>
+      </x:c>
+      <x:c r="E12" s="1" t="str">
+        <x:v>(111)333111</x:v>
+      </x:c>
+      <x:c r="F12" s="4" t="n">
+        <x:v>1988</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13">
+      <x:c r="A13" s="4" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B13" s="1" t="str">
+        <x:v>Witcher</x:v>
+      </x:c>
+      <x:c r="C13" s="1" t="str">
+        <x:v>Moon</x:v>
+      </x:c>
+      <x:c r="D13" s="1" t="str">
+        <x:v>witcher@gmail.com</x:v>
+      </x:c>
+      <x:c r="E13" s="1" t="str">
+        <x:v>(111)333999</x:v>
+      </x:c>
+      <x:c r="F13" s="4" t="n">
+        <x:v>1990</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14">
+      <x:c r="A14" s="4" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B14" s="1" t="str">
+        <x:v>Supwom</x:v>
+      </x:c>
+      <x:c r="C14" s="1" t="str">
+        <x:v>Nanual</x:v>
+      </x:c>
+      <x:c r="D14" s="1" t="str">
+        <x:v>supwom@gmail.com</x:v>
+      </x:c>
+      <x:c r="E14" s="1" t="str">
+        <x:v>(111)333777</x:v>
+      </x:c>
+      <x:c r="F14" s="4" t="n">
+        <x:v>1988</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15">
+      <x:c r="A15" s="4" t="n">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B15" s="1" t="str">
+        <x:v>User5</x:v>
+      </x:c>
+      <x:c r="C15" s="1" t="str">
+        <x:v>User5LN</x:v>
+      </x:c>
+      <x:c r="D15" s="1" t="str">
+        <x:v>user5@gmail.com</x:v>
+      </x:c>
+      <x:c r="E15" s="1" t="str">
+        <x:v/>
+      </x:c>
+      <x:c r="F15" s="4" t="n">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16">
+      <x:c r="A16" s="4" t="n">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B16" s="1" t="str">
+        <x:v>Barney</x:v>
+      </x:c>
+      <x:c r="C16" s="1" t="str">
+        <x:v>Ross</x:v>
+      </x:c>
+      <x:c r="D16" s="1" t="str">
+        <x:v>barney@gmail.com</x:v>
+      </x:c>
+      <x:c r="E16" s="1" t="str">
+        <x:v>(111)222333</x:v>
+      </x:c>
+      <x:c r="F16" s="4" t="n">
+        <x:v>1975</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17">
+      <x:c r="A17" s="4" t="n">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B17" s="1" t="str">
+        <x:v>User2</x:v>
+      </x:c>
+      <x:c r="C17" s="1" t="str">
+        <x:v>User2LN</x:v>
+      </x:c>
+      <x:c r="D17" s="1" t="str">
+        <x:v>user2@gmail.com</x:v>
+      </x:c>
+      <x:c r="E17" s="1" t="str">
+        <x:v>(123)123123</x:v>
+      </x:c>
+      <x:c r="F17" s="4" t="n">
+        <x:v>1995</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18">
+      <x:c r="A18" s="4" t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B18" s="1" t="str">
+        <x:v>Lee</x:v>
+      </x:c>
+      <x:c r="C18" s="1" t="str">
+        <x:v>Christmas</x:v>
+      </x:c>
+      <x:c r="D18" s="1" t="str">
+        <x:v>lee@gmail.com</x:v>
+      </x:c>
+      <x:c r="E18" s="1" t="str">
+        <x:v>(111)333444</x:v>
+      </x:c>
+      <x:c r="F18" s="4" t="n">
+        <x:v>1977</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19">
+      <x:c r="A19" s="4" t="n">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B19" s="1" t="str">
+        <x:v>User3</x:v>
+      </x:c>
+      <x:c r="C19" s="1" t="str">
+        <x:v>User3LN</x:v>
+      </x:c>
+      <x:c r="D19" s="1" t="str">
+        <x:v>user3@gmail.com</x:v>
+      </x:c>
+      <x:c r="E19" s="1" t="str">
+        <x:v>(123)123124</x:v>
+      </x:c>
+      <x:c r="F19" s="4" t="n">
+        <x:v>1996</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20">
+      <x:c r="A20" s="4" t="n">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B20" s="1" t="str">
+        <x:v>Marvel</x:v>
+      </x:c>
+      <x:c r="C20" s="1" t="str">
+        <x:v>Levram</x:v>
+      </x:c>
+      <x:c r="D20" s="1" t="str">
+        <x:v>marvel@gmail.com</x:v>
+      </x:c>
+      <x:c r="E20" s="1" t="str">
+        <x:v>(111)333555</x:v>
+      </x:c>
+      <x:c r="F20" s="4" t="n">
+        <x:v>1995</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21">
+      <x:c r="A21" s="4" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B21" s="1" t="str">
+        <x:v>Jean</x:v>
+      </x:c>
+      <x:c r="C21" s="1" t="str">
+        <x:v>Vilain</x:v>
+      </x:c>
+      <x:c r="D21" s="1" t="str">
+        <x:v>jean@gmail.com</x:v>
+      </x:c>
+      <x:c r="E21" s="1" t="str">
+        <x:v>(111)222777</x:v>
+      </x:c>
+      <x:c r="F21" s="4" t="n">
+        <x:v>1973</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22">
+      <x:c r="A22" s="4" t="n">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B22" s="1" t="str">
         <x:v>Sonya</x:v>
       </x:c>
-      <x:c r="C4" s="1" t="str">
+      <x:c r="C22" s="1" t="str">
         <x:v>Night</x:v>
       </x:c>
-      <x:c r="D4" s="1" t="str">
+      <x:c r="D22" s="1" t="str">
         <x:v>sonya@gmail.com</x:v>
       </x:c>
-      <x:c r="E4" s="1" t="str">
+      <x:c r="E22" s="1" t="str">
         <x:v>(111)333666</x:v>
       </x:c>
-      <x:c r="F4" s="4" t="n">
+      <x:c r="F22" s="4" t="n">
         <x:v>1996</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23">
+      <x:c r="A23" s="4" t="n">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B23" s="1" t="str">
+        <x:v>Natalia</x:v>
+      </x:c>
+      <x:c r="C23" s="1" t="str">
+        <x:v>Romanoff</x:v>
+      </x:c>
+      <x:c r="D23" s="1" t="str">
+        <x:v>natalia@gmail.com</x:v>
+      </x:c>
+      <x:c r="E23" s="1" t="str">
+        <x:v>(111)222888</x:v>
+      </x:c>
+      <x:c r="F23" s="4" t="n">
+        <x:v>1986</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Async/await refactoring (!ExcelService implementations)
</commit_message>
<xml_diff>
--- a/FitMeApp/wwwroot/ExcelFiles/Users.xlsx
+++ b/FitMeApp/wwwroot/ExcelFiles/Users.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users.xlsx" sheetId="1" r:id="Rc5b5b1147a1c434f"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Users.xlsx" sheetId="1" r:id="Rb3d452f3c886457f"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -288,19 +288,19 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B11" s="1" t="str">
-        <x:v>Bruce</x:v>
+        <x:v>User8</x:v>
       </x:c>
       <x:c r="C11" s="1" t="str">
-        <x:v>Lee</x:v>
+        <x:v>User8LN</x:v>
       </x:c>
       <x:c r="D11" s="1" t="str">
-        <x:v>bruce@gmail.com</x:v>
+        <x:v>user8@gmail.com</x:v>
       </x:c>
       <x:c r="E11" s="1" t="str">
-        <x:v>(111)333445</x:v>
+        <x:v/>
       </x:c>
       <x:c r="F11" s="4" t="n">
-        <x:v>1987</x:v>
+        <x:v>2000</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
@@ -308,19 +308,19 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="B12" s="1" t="str">
-        <x:v>Gamora</x:v>
+        <x:v>Bruce</x:v>
       </x:c>
       <x:c r="C12" s="1" t="str">
-        <x:v>Gamorak</x:v>
+        <x:v>Lee</x:v>
       </x:c>
       <x:c r="D12" s="1" t="str">
-        <x:v>gamora@gmail.com</x:v>
+        <x:v>bruce@gmail.com</x:v>
       </x:c>
       <x:c r="E12" s="1" t="str">
-        <x:v>(111)333111</x:v>
+        <x:v>(111)333445</x:v>
       </x:c>
       <x:c r="F12" s="4" t="n">
-        <x:v>1988</x:v>
+        <x:v>1987</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
@@ -328,19 +328,19 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="B13" s="1" t="str">
-        <x:v>Witcher</x:v>
+        <x:v>Gamora</x:v>
       </x:c>
       <x:c r="C13" s="1" t="str">
-        <x:v>Moon</x:v>
+        <x:v>Gamorak</x:v>
       </x:c>
       <x:c r="D13" s="1" t="str">
-        <x:v>witcher@gmail.com</x:v>
+        <x:v>gamora@gmail.com</x:v>
       </x:c>
       <x:c r="E13" s="1" t="str">
-        <x:v>(111)333999</x:v>
+        <x:v>(111)333111</x:v>
       </x:c>
       <x:c r="F13" s="4" t="n">
-        <x:v>1990</x:v>
+        <x:v>1988</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
@@ -348,19 +348,19 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="B14" s="1" t="str">
-        <x:v>Supwom</x:v>
+        <x:v>Witcher</x:v>
       </x:c>
       <x:c r="C14" s="1" t="str">
-        <x:v>Nanual</x:v>
+        <x:v>Moon</x:v>
       </x:c>
       <x:c r="D14" s="1" t="str">
-        <x:v>supwom@gmail.com</x:v>
+        <x:v>witcher@gmail.com</x:v>
       </x:c>
       <x:c r="E14" s="1" t="str">
-        <x:v>(111)333777</x:v>
+        <x:v>(111)333999</x:v>
       </x:c>
       <x:c r="F14" s="4" t="n">
-        <x:v>1988</x:v>
+        <x:v>1990</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
@@ -368,19 +368,19 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="B15" s="1" t="str">
-        <x:v>User5</x:v>
+        <x:v>Supwom</x:v>
       </x:c>
       <x:c r="C15" s="1" t="str">
-        <x:v>User5LN</x:v>
+        <x:v>Nanual</x:v>
       </x:c>
       <x:c r="D15" s="1" t="str">
-        <x:v>user5@gmail.com</x:v>
+        <x:v>supwom@gmail.com</x:v>
       </x:c>
       <x:c r="E15" s="1" t="str">
-        <x:v/>
+        <x:v>(111)333777</x:v>
       </x:c>
       <x:c r="F15" s="4" t="n">
-        <x:v>0</x:v>
+        <x:v>1988</x:v>
       </x:c>
     </x:row>
     <x:row r="16">

</xml_diff>